<commit_message>
started work on multiple regression
</commit_message>
<xml_diff>
--- a/raster-data-key.xlsx
+++ b/raster-data-key.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t xml:space="preserve">parameter</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">CHELSA_bio3_1981-2010_V.2.1.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">temperature seasonality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHELSA_bio4_1981-2010_V.2.1.tif</t>
   </si>
   <si>
     <t xml:space="preserve">annual precipitation</t>
@@ -286,10 +280,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,7 +437,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -463,7 +457,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -471,36 +465,36 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>32767</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
+      <c r="D10" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>32767</v>
+        <v>-9999</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -509,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>27</v>
@@ -529,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>29</v>
@@ -549,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>31</v>
@@ -569,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>33</v>
@@ -589,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>35</v>
@@ -609,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>37</v>
@@ -629,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>39</v>
@@ -649,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>41</v>
@@ -669,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>43</v>
@@ -689,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>45</v>
@@ -709,32 +703,12 @@
         <v>0</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="0" t="n">
         <v>-9999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created control variable collation script
</commit_message>
<xml_diff>
--- a/raster-data-key.xlsx
+++ b/raster-data-key.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">mean annual temp</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/mcoving/Dropbox/sync/projects/Dolines/comparison_data/chelsa_v2/envicloud/chelsa/chelsa_V2/GLOBAL/climatologies/1981-2010/bio/</t>
+    <t xml:space="preserve">./comparison-datasets/chelsa_v2/envicloud/chelsa/chelsa_V2/GLOBAL/climatologies/1981-2010/bio/</t>
   </si>
   <si>
     <t xml:space="preserve">CHELSA_bio1_1981-2010_V.2.1.tif</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">carbonate</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/mcoving/Dropbox/sync/projects/Dolines/comparison_data/gNATSGO/UC-Davis-agg</t>
+    <t xml:space="preserve">./comparison-datasets/UC-Davis-soil-properties/</t>
   </si>
   <si>
     <t xml:space="preserve">caco3_kg_sq_m.tif</t>
@@ -283,7 +283,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -312,7 +312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -332,7 +332,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
@@ -352,7 +352,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
@@ -372,7 +372,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -392,7 +392,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>15</v>
       </c>
@@ -412,7 +412,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>17</v>
       </c>
@@ -432,7 +432,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
@@ -452,7 +452,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>

</xml_diff>